<commit_message>
use identifier/source field as unique_together
</commit_message>
<xml_diff>
--- a/backend/data/testdata/SampleData.xlsx
+++ b/backend/data/testdata/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berit/git-uu/jewish-historical-migration/backend/data/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F38FAFC7-54ED-7A48-8EA8-56874A321037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E10CA7D-968C-7846-ADA0-CF1C09280044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="1520" windowWidth="27640" windowHeight="16620" activeTab="1" xr2:uid="{75BA4E8E-4E5F-6542-ACD0-DA59D4501059}"/>
+    <workbookView xWindow="-28380" yWindow="1520" windowWidth="27640" windowHeight="16620" xr2:uid="{75BA4E8E-4E5F-6542-ACD0-DA59D4501059}"/>
   </bookViews>
   <sheets>
     <sheet name="Data MJHM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -57,12 +57,6 @@
     <t xml:space="preserve">own id </t>
   </si>
   <si>
-    <t>type1</t>
-  </si>
-  <si>
-    <t>type2</t>
-  </si>
-  <si>
     <t>period</t>
   </si>
   <si>
@@ -199,6 +193,27 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>category 1</t>
+  </si>
+  <si>
+    <t>category 2</t>
+  </si>
+  <si>
+    <t>mention religious profession</t>
+  </si>
+  <si>
+    <t>sexe dedicator epitaph (male/female/child)</t>
+  </si>
+  <si>
+    <t>sexe of deceased (male/female/child)</t>
+  </si>
+  <si>
+    <t>Child (Male)</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -605,15 +620,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1770E8F-7467-1141-BFB8-408817C67F28}">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,124 +648,137 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="V1" s="4"/>
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="6">
         <v>315199</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="K2" s="6">
         <v>1</v>
       </c>
       <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="T2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
         <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
       </c>
       <c r="J3" s="6">
         <v>4</v>
@@ -759,52 +787,52 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" t="s">
         <v>36</v>
       </c>
-      <c r="O3" t="s">
+      <c r="W3" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6">
         <v>305064</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J4" s="6">
         <v>4</v>
@@ -813,22 +841,28 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" t="s">
         <v>41</v>
       </c>
-      <c r="O4" t="s">
+      <c r="W4" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="R4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC68684C-EB31-D14D-91B9-B96EE94C4116}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -854,56 +888,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>